<commit_message>
Ignore changes to excel file
ignore changes to the excel file
</commit_message>
<xml_diff>
--- a/AD_Group_Comparison.xlsx
+++ b/AD_Group_Comparison.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gzxvand\Documents\GitHub\active-directory-group-comparison\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EE7DF5E-0465-4293-BEDA-2DD896538544}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F8687A4-0FFD-4C7B-A74D-8B0A33A4B1C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>AD Group 1</t>
   </si>
@@ -28,19 +28,10 @@
     <t>AD Group 2</t>
   </si>
   <si>
-    <t>GrpGIT_Mobilitas_Write</t>
+    <t>GrpGWGCC_LOG_Admins</t>
   </si>
   <si>
-    <t>GrpGWGCC_SM_Prod_Admins</t>
-  </si>
-  <si>
-    <t>GrpGWGCC_SM_Admins</t>
-  </si>
-  <si>
-    <t>GrpGWGCC_SCM_Users</t>
-  </si>
-  <si>
-    <t>GrpGWGCC_LOG_Admins</t>
+    <t>GrpGWGCC_LOG_Users</t>
   </si>
 </sst>
 </file>
@@ -408,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -435,30 +426,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated the script to v3 to also pull a list of AD Groups a list of provided users are  part of. The new excel file it reads from is v2.
</commit_message>
<xml_diff>
--- a/AD_Group_Comparison.xlsx
+++ b/AD_Group_Comparison.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gzxvand\Documents\GitHub\active-directory-group-comparison\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F8687A4-0FFD-4C7B-A74D-8B0A33A4B1C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DED55C00-9B60-4A90-8F13-E2C77E9B537C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Comparison Results" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
   <si>
     <t>AD Group 1</t>
   </si>
@@ -32,6 +33,21 @@
   </si>
   <si>
     <t>GrpGWGCC_LOG_Users</t>
+  </si>
+  <si>
+    <t>Comparison Results</t>
+  </si>
+  <si>
+    <t>Timestamp</t>
+  </si>
+  <si>
+    <t>Ramachandran, Hemanathan (g2gyram) (g2gyram); Ramalingam, Karthikeyan (e0hrama) (e0hrama)</t>
+  </si>
+  <si>
+    <t>2024-09-24 13:54:04</t>
+  </si>
+  <si>
+    <t>2024-09-24 14:02:15</t>
   </si>
 </sst>
 </file>
@@ -401,7 +417,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -431,6 +447,69 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A2:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="87.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{2d48d056-9dcf-480d-be28-f64a2de71bca}" enabled="1" method="Standard" siteId="{1345b410-9694-46f3-9c42-132a582646b5}" contentBits="0" removed="0"/>

</xml_diff>